<commit_message>
Updated sprintbacklog with status
</commit_message>
<xml_diff>
--- a/Sprint_2/Sprint_Backlog/SprintBacklog2.xlsx
+++ b/Sprint_2/Sprint_Backlog/SprintBacklog2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\AC31007\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\AC31007\team5agile\Sprint_2\Sprint_Backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="33">
   <si>
     <t>User Story #1</t>
   </si>
@@ -96,12 +96,6 @@
     <t>Date Added</t>
   </si>
   <si>
-    <t>As a application user, I want to be ale to set a constraint based on my set location</t>
-  </si>
-  <si>
-    <t>As an application user, I want to be ale to set a constraint based on my set price range.</t>
-  </si>
-  <si>
     <t>As an application user, I want to be able to order my results based on price.</t>
   </si>
   <si>
@@ -121,6 +115,15 @@
   </si>
   <si>
     <t>As a user, I want to be able to load new/edited data to delete from existing data set</t>
+  </si>
+  <si>
+    <t>As a application user, I want to be able to set a constraint based on my set location</t>
+  </si>
+  <si>
+    <t>As an application user, I want to be able to set a constraint based on my set price range.</t>
+  </si>
+  <si>
+    <t>Incomplete</t>
   </si>
 </sst>
 </file>
@@ -337,14 +340,6 @@
     <xf numFmtId="14" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -360,6 +355,14 @@
     <xf numFmtId="14" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -1285,7 +1288,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -1308,30 +1311,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:29" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="18"/>
-      <c r="R1" s="18"/>
-      <c r="S1" s="18"/>
-      <c r="T1" s="18"/>
-      <c r="U1" s="18"/>
-      <c r="V1" s="18"/>
-      <c r="W1" s="18"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
+      <c r="Q1" s="23"/>
+      <c r="R1" s="23"/>
+      <c r="S1" s="23"/>
+      <c r="T1" s="23"/>
+      <c r="U1" s="23"/>
+      <c r="V1" s="23"/>
+      <c r="W1" s="23"/>
       <c r="X1" s="4"/>
       <c r="Y1" s="4"/>
       <c r="Z1" s="4"/>
@@ -1394,17 +1397,19 @@
       <c r="AC2" s="4"/>
     </row>
     <row r="3" spans="2:29" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="24">
+      <c r="B3" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="20">
         <v>2</v>
       </c>
-      <c r="D3" s="25">
+      <c r="D3" s="21">
         <v>43864</v>
       </c>
       <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
+      <c r="F3" s="17" t="s">
+        <v>32</v>
+      </c>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
       <c r="I3" s="12"/>
@@ -1434,7 +1439,9 @@
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
+      <c r="F4" s="9" t="s">
+        <v>32</v>
+      </c>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
       <c r="I4" s="9"/>
@@ -1466,7 +1473,9 @@
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
+      <c r="F5" s="9" t="s">
+        <v>32</v>
+      </c>
       <c r="G5" s="9"/>
       <c r="H5" s="9"/>
       <c r="I5" s="9"/>
@@ -1498,7 +1507,9 @@
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
+      <c r="F6" s="9" t="s">
+        <v>32</v>
+      </c>
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
@@ -1526,17 +1537,19 @@
       <c r="AC6" s="4"/>
     </row>
     <row r="7" spans="2:29" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="24">
+      <c r="B7" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="20">
         <v>2</v>
       </c>
-      <c r="D7" s="25">
+      <c r="D7" s="21">
         <v>43864</v>
       </c>
       <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
+      <c r="F7" s="17" t="s">
+        <v>32</v>
+      </c>
       <c r="G7" s="12"/>
       <c r="H7" s="12"/>
       <c r="I7" s="12"/>
@@ -1566,7 +1579,9 @@
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
+      <c r="F8" s="9" t="s">
+        <v>32</v>
+      </c>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
@@ -1598,7 +1613,9 @@
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
+      <c r="F9" s="9" t="s">
+        <v>32</v>
+      </c>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
@@ -1626,17 +1643,19 @@
       <c r="AC9" s="4"/>
     </row>
     <row r="10" spans="2:29" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="24">
+      <c r="B10" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="20">
         <v>1</v>
       </c>
-      <c r="D10" s="25">
+      <c r="D10" s="21">
         <v>43864</v>
       </c>
       <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
+      <c r="F10" s="17" t="s">
+        <v>32</v>
+      </c>
       <c r="G10" s="12"/>
       <c r="H10" s="12"/>
       <c r="I10" s="12"/>
@@ -1666,7 +1685,9 @@
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
+      <c r="F11" s="9" t="s">
+        <v>32</v>
+      </c>
       <c r="G11" s="9"/>
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
@@ -1698,7 +1719,9 @@
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
+      <c r="F12" s="9" t="s">
+        <v>32</v>
+      </c>
       <c r="G12" s="9"/>
       <c r="H12" s="9"/>
       <c r="I12" s="9"/>
@@ -1730,7 +1753,9 @@
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
+      <c r="F13" s="9" t="s">
+        <v>32</v>
+      </c>
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
       <c r="I13" s="9"/>
@@ -1762,7 +1787,9 @@
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
+      <c r="F14" s="9" t="s">
+        <v>32</v>
+      </c>
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
       <c r="I14" s="9"/>
@@ -1790,17 +1817,19 @@
       <c r="AC14" s="4"/>
     </row>
     <row r="15" spans="2:29" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="24">
+      <c r="B15" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="20">
         <v>1</v>
       </c>
-      <c r="D15" s="25">
+      <c r="D15" s="21">
         <v>43864</v>
       </c>
       <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
+      <c r="F15" s="17" t="s">
+        <v>32</v>
+      </c>
       <c r="G15" s="12"/>
       <c r="H15" s="12"/>
       <c r="I15" s="12"/>
@@ -1830,7 +1859,9 @@
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
+      <c r="F16" s="9" t="s">
+        <v>32</v>
+      </c>
       <c r="G16" s="9"/>
       <c r="H16" s="9"/>
       <c r="I16" s="9"/>
@@ -1862,7 +1893,9 @@
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
       <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
+      <c r="F17" s="9" t="s">
+        <v>32</v>
+      </c>
       <c r="G17" s="9"/>
       <c r="H17" s="9"/>
       <c r="I17" s="9"/>
@@ -1894,7 +1927,9 @@
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
+      <c r="F18" s="9" t="s">
+        <v>32</v>
+      </c>
       <c r="G18" s="9"/>
       <c r="H18" s="9"/>
       <c r="I18" s="9"/>
@@ -1926,7 +1961,9 @@
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
+      <c r="F19" s="9" t="s">
+        <v>32</v>
+      </c>
       <c r="G19" s="9"/>
       <c r="H19" s="9"/>
       <c r="I19" s="9"/>
@@ -1954,17 +1991,19 @@
       <c r="AC19" s="4"/>
     </row>
     <row r="20" spans="2:29" s="13" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" s="21">
+      <c r="B20" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="17">
         <v>2</v>
       </c>
       <c r="D20" s="16">
         <v>43864</v>
       </c>
       <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
+      <c r="F20" s="17" t="s">
+        <v>32</v>
+      </c>
       <c r="G20" s="12"/>
       <c r="H20" s="12"/>
       <c r="I20" s="12"/>
@@ -1978,7 +2017,9 @@
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
       <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
+      <c r="F21" s="9" t="s">
+        <v>32</v>
+      </c>
       <c r="G21" s="9"/>
       <c r="H21" s="9"/>
       <c r="I21" s="9"/>
@@ -2010,7 +2051,9 @@
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
       <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
+      <c r="F22" s="9" t="s">
+        <v>32</v>
+      </c>
       <c r="G22" s="9"/>
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>
@@ -2038,17 +2081,19 @@
       <c r="AC22" s="4"/>
     </row>
     <row r="23" spans="2:29" s="13" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="C23" s="21">
+      <c r="B23" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="17">
         <v>4</v>
       </c>
       <c r="D23" s="16">
         <v>43864</v>
       </c>
       <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
+      <c r="F23" s="17" t="s">
+        <v>32</v>
+      </c>
       <c r="G23" s="12"/>
       <c r="H23" s="12"/>
       <c r="I23" s="12"/>
@@ -2062,7 +2107,9 @@
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
       <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
+      <c r="F24" s="9" t="s">
+        <v>32</v>
+      </c>
       <c r="G24" s="9"/>
       <c r="H24" s="9"/>
       <c r="I24" s="9"/>
@@ -2094,7 +2141,9 @@
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
       <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
+      <c r="F25" s="9" t="s">
+        <v>32</v>
+      </c>
       <c r="G25" s="9"/>
       <c r="H25" s="9"/>
       <c r="I25" s="9"/>
@@ -2126,7 +2175,9 @@
       <c r="C26" s="9"/>
       <c r="D26" s="9"/>
       <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
+      <c r="F26" s="9" t="s">
+        <v>32</v>
+      </c>
       <c r="G26" s="9"/>
       <c r="H26" s="9"/>
       <c r="I26" s="9"/>
@@ -2158,7 +2209,9 @@
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
       <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
+      <c r="F27" s="9" t="s">
+        <v>32</v>
+      </c>
       <c r="G27" s="9"/>
       <c r="H27" s="9"/>
       <c r="I27" s="9"/>
@@ -2186,17 +2239,19 @@
       <c r="AC27" s="4"/>
     </row>
     <row r="28" spans="2:29" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="C28" s="21">
+      <c r="B28" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" s="17">
         <v>5</v>
       </c>
       <c r="D28" s="16">
         <v>43864</v>
       </c>
       <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
+      <c r="F28" s="17" t="s">
+        <v>32</v>
+      </c>
       <c r="G28" s="12"/>
       <c r="H28" s="12"/>
       <c r="I28" s="12"/>
@@ -2226,7 +2281,9 @@
       <c r="C29" s="15"/>
       <c r="D29" s="15"/>
       <c r="E29" s="9"/>
-      <c r="F29" s="14"/>
+      <c r="F29" s="9" t="s">
+        <v>32</v>
+      </c>
       <c r="G29" s="14"/>
       <c r="H29" s="14"/>
       <c r="I29" s="14"/>
@@ -2258,7 +2315,9 @@
       <c r="C30" s="9"/>
       <c r="D30" s="9"/>
       <c r="E30" s="9"/>
-      <c r="F30" s="9"/>
+      <c r="F30" s="9" t="s">
+        <v>32</v>
+      </c>
       <c r="G30" s="9"/>
       <c r="H30" s="9"/>
       <c r="I30" s="9"/>
@@ -2286,17 +2345,19 @@
       <c r="AC30" s="4"/>
     </row>
     <row r="31" spans="2:29" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="C31" s="21">
+      <c r="B31" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C31" s="17">
         <v>5</v>
       </c>
       <c r="D31" s="16">
         <v>43864</v>
       </c>
       <c r="E31" s="12"/>
-      <c r="F31" s="12"/>
+      <c r="F31" s="17" t="s">
+        <v>32</v>
+      </c>
       <c r="G31" s="12"/>
       <c r="H31" s="12"/>
       <c r="I31" s="12"/>
@@ -2326,7 +2387,9 @@
       <c r="C32" s="9"/>
       <c r="D32" s="9"/>
       <c r="E32" s="9"/>
-      <c r="F32" s="9"/>
+      <c r="F32" s="9" t="s">
+        <v>32</v>
+      </c>
       <c r="G32" s="9"/>
       <c r="H32" s="9"/>
       <c r="I32" s="9"/>
@@ -2354,11 +2417,13 @@
       <c r="AC32" s="4"/>
     </row>
     <row r="33" spans="2:29" s="13" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="22"/>
-      <c r="C33" s="22"/>
-      <c r="D33" s="23"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="19"/>
       <c r="E33" s="14"/>
-      <c r="F33" s="14"/>
+      <c r="F33" s="9" t="s">
+        <v>32</v>
+      </c>
       <c r="G33" s="14"/>
       <c r="H33" s="14"/>
       <c r="I33" s="14"/>
@@ -2370,17 +2435,19 @@
       </c>
     </row>
     <row r="34" spans="2:29" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="C34" s="21">
+      <c r="B34" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C34" s="17">
         <v>5</v>
       </c>
       <c r="D34" s="16">
         <v>43864</v>
       </c>
       <c r="E34" s="12"/>
-      <c r="F34" s="12"/>
+      <c r="F34" s="17" t="s">
+        <v>32</v>
+      </c>
       <c r="G34" s="12"/>
       <c r="H34" s="12"/>
       <c r="I34" s="12"/>
@@ -2410,7 +2477,9 @@
       <c r="C35" s="9"/>
       <c r="D35" s="9"/>
       <c r="E35" s="9"/>
-      <c r="F35" s="9"/>
+      <c r="F35" s="9" t="s">
+        <v>32</v>
+      </c>
       <c r="G35" s="9"/>
       <c r="H35" s="9"/>
       <c r="I35" s="9"/>
@@ -2442,7 +2511,9 @@
       <c r="C36" s="9"/>
       <c r="D36" s="9"/>
       <c r="E36" s="9"/>
-      <c r="F36" s="9"/>
+      <c r="F36" s="9" t="s">
+        <v>32</v>
+      </c>
       <c r="G36" s="9"/>
       <c r="H36" s="9"/>
       <c r="I36" s="9"/>
@@ -2553,30 +2624,30 @@
       <c r="AC38" s="4"/>
     </row>
     <row r="39" spans="2:29" ht="49.9" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B39" s="19" t="s">
+      <c r="B39" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="C39" s="20"/>
-      <c r="D39" s="20"/>
-      <c r="E39" s="20"/>
-      <c r="F39" s="20"/>
-      <c r="G39" s="20"/>
-      <c r="H39" s="20"/>
-      <c r="I39" s="20"/>
-      <c r="J39" s="20"/>
-      <c r="K39" s="20"/>
-      <c r="L39" s="20"/>
-      <c r="M39" s="20"/>
-      <c r="N39" s="20"/>
-      <c r="O39" s="20"/>
-      <c r="P39" s="20"/>
-      <c r="Q39" s="20"/>
-      <c r="R39" s="20"/>
-      <c r="S39" s="20"/>
-      <c r="T39" s="20"/>
-      <c r="U39" s="20"/>
-      <c r="V39" s="20"/>
-      <c r="W39" s="20"/>
+      <c r="C39" s="25"/>
+      <c r="D39" s="25"/>
+      <c r="E39" s="25"/>
+      <c r="F39" s="25"/>
+      <c r="G39" s="25"/>
+      <c r="H39" s="25"/>
+      <c r="I39" s="25"/>
+      <c r="J39" s="25"/>
+      <c r="K39" s="25"/>
+      <c r="L39" s="25"/>
+      <c r="M39" s="25"/>
+      <c r="N39" s="25"/>
+      <c r="O39" s="25"/>
+      <c r="P39" s="25"/>
+      <c r="Q39" s="25"/>
+      <c r="R39" s="25"/>
+      <c r="S39" s="25"/>
+      <c r="T39" s="25"/>
+      <c r="U39" s="25"/>
+      <c r="V39" s="25"/>
+      <c r="W39" s="25"/>
       <c r="X39" s="4"/>
       <c r="Y39" s="4"/>
       <c r="Z39" s="4"/>
@@ -5450,29 +5521,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:28" ht="49.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="18"/>
-      <c r="R1" s="18"/>
-      <c r="S1" s="18"/>
-      <c r="T1" s="18"/>
-      <c r="U1" s="18"/>
-      <c r="V1" s="18"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
+      <c r="Q1" s="23"/>
+      <c r="R1" s="23"/>
+      <c r="S1" s="23"/>
+      <c r="T1" s="23"/>
+      <c r="U1" s="23"/>
+      <c r="V1" s="23"/>
       <c r="W1" s="4"/>
       <c r="X1" s="4"/>
       <c r="Y1" s="4"/>

</xml_diff>

<commit_message>
Adding Sprint Backlog 2 with tasks and base to Documentation
</commit_message>
<xml_diff>
--- a/Sprint_2/Sprint_Backlog/SprintBacklog2.xlsx
+++ b/Sprint_2/Sprint_Backlog/SprintBacklog2.xlsx
@@ -1287,8 +1287,8 @@
   <dimension ref="B1:AC133"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G35" sqref="G35:L36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -1442,12 +1442,24 @@
       <c r="F4" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
+      <c r="G4" s="9">
+        <v>0</v>
+      </c>
+      <c r="H4" s="9">
+        <v>0</v>
+      </c>
+      <c r="I4" s="9">
+        <v>0</v>
+      </c>
+      <c r="J4" s="9">
+        <v>0</v>
+      </c>
+      <c r="K4" s="9">
+        <v>0</v>
+      </c>
+      <c r="L4" s="9">
+        <v>0</v>
+      </c>
       <c r="M4" s="9">
         <v>0</v>
       </c>
@@ -1476,12 +1488,24 @@
       <c r="F5" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9"/>
+      <c r="G5" s="9">
+        <v>0</v>
+      </c>
+      <c r="H5" s="9">
+        <v>0</v>
+      </c>
+      <c r="I5" s="9">
+        <v>0</v>
+      </c>
+      <c r="J5" s="9">
+        <v>0</v>
+      </c>
+      <c r="K5" s="9">
+        <v>0</v>
+      </c>
+      <c r="L5" s="9">
+        <v>0</v>
+      </c>
       <c r="M5" s="9">
         <v>0</v>
       </c>
@@ -1510,12 +1534,24 @@
       <c r="F6" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9"/>
+      <c r="G6" s="9">
+        <v>0</v>
+      </c>
+      <c r="H6" s="9">
+        <v>0</v>
+      </c>
+      <c r="I6" s="9">
+        <v>0</v>
+      </c>
+      <c r="J6" s="9">
+        <v>0</v>
+      </c>
+      <c r="K6" s="9">
+        <v>0</v>
+      </c>
+      <c r="L6" s="9">
+        <v>0</v>
+      </c>
       <c r="M6" s="9">
         <v>0</v>
       </c>
@@ -1582,12 +1618,24 @@
       <c r="F8" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
+      <c r="G8" s="9">
+        <v>0</v>
+      </c>
+      <c r="H8" s="9">
+        <v>0</v>
+      </c>
+      <c r="I8" s="9">
+        <v>0</v>
+      </c>
+      <c r="J8" s="9">
+        <v>0</v>
+      </c>
+      <c r="K8" s="9">
+        <v>0</v>
+      </c>
+      <c r="L8" s="9">
+        <v>0</v>
+      </c>
       <c r="M8" s="9">
         <v>0</v>
       </c>
@@ -1616,12 +1664,24 @@
       <c r="F9" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="9"/>
+      <c r="G9" s="9">
+        <v>0</v>
+      </c>
+      <c r="H9" s="9">
+        <v>0</v>
+      </c>
+      <c r="I9" s="9">
+        <v>0</v>
+      </c>
+      <c r="J9" s="9">
+        <v>0</v>
+      </c>
+      <c r="K9" s="9">
+        <v>0</v>
+      </c>
+      <c r="L9" s="9">
+        <v>0</v>
+      </c>
       <c r="M9" s="9">
         <v>0</v>
       </c>
@@ -1688,12 +1748,24 @@
       <c r="F11" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
+      <c r="G11" s="9">
+        <v>0</v>
+      </c>
+      <c r="H11" s="9">
+        <v>0</v>
+      </c>
+      <c r="I11" s="9">
+        <v>0</v>
+      </c>
+      <c r="J11" s="9">
+        <v>0</v>
+      </c>
+      <c r="K11" s="9">
+        <v>0</v>
+      </c>
+      <c r="L11" s="9">
+        <v>0</v>
+      </c>
       <c r="M11" s="9">
         <v>0</v>
       </c>
@@ -1722,12 +1794,24 @@
       <c r="F12" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9"/>
+      <c r="G12" s="9">
+        <v>0</v>
+      </c>
+      <c r="H12" s="9">
+        <v>0</v>
+      </c>
+      <c r="I12" s="9">
+        <v>0</v>
+      </c>
+      <c r="J12" s="9">
+        <v>0</v>
+      </c>
+      <c r="K12" s="9">
+        <v>0</v>
+      </c>
+      <c r="L12" s="9">
+        <v>0</v>
+      </c>
       <c r="M12" s="9">
         <v>0</v>
       </c>
@@ -1756,12 +1840,24 @@
       <c r="F13" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="9"/>
+      <c r="G13" s="9">
+        <v>0</v>
+      </c>
+      <c r="H13" s="9">
+        <v>0</v>
+      </c>
+      <c r="I13" s="9">
+        <v>0</v>
+      </c>
+      <c r="J13" s="9">
+        <v>0</v>
+      </c>
+      <c r="K13" s="9">
+        <v>0</v>
+      </c>
+      <c r="L13" s="9">
+        <v>0</v>
+      </c>
       <c r="M13" s="9">
         <v>0</v>
       </c>
@@ -1790,12 +1886,24 @@
       <c r="F14" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="9"/>
-      <c r="L14" s="9"/>
+      <c r="G14" s="9">
+        <v>0</v>
+      </c>
+      <c r="H14" s="9">
+        <v>0</v>
+      </c>
+      <c r="I14" s="9">
+        <v>0</v>
+      </c>
+      <c r="J14" s="9">
+        <v>0</v>
+      </c>
+      <c r="K14" s="9">
+        <v>0</v>
+      </c>
+      <c r="L14" s="9">
+        <v>0</v>
+      </c>
       <c r="M14" s="9">
         <v>0</v>
       </c>
@@ -1862,12 +1970,24 @@
       <c r="F16" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="9"/>
-      <c r="L16" s="9"/>
+      <c r="G16" s="9">
+        <v>0</v>
+      </c>
+      <c r="H16" s="9">
+        <v>0</v>
+      </c>
+      <c r="I16" s="9">
+        <v>0</v>
+      </c>
+      <c r="J16" s="9">
+        <v>0</v>
+      </c>
+      <c r="K16" s="9">
+        <v>0</v>
+      </c>
+      <c r="L16" s="9">
+        <v>0</v>
+      </c>
       <c r="M16" s="9">
         <v>0</v>
       </c>
@@ -1896,12 +2016,24 @@
       <c r="F17" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
-      <c r="L17" s="9"/>
+      <c r="G17" s="9">
+        <v>0</v>
+      </c>
+      <c r="H17" s="9">
+        <v>0</v>
+      </c>
+      <c r="I17" s="9">
+        <v>0</v>
+      </c>
+      <c r="J17" s="9">
+        <v>0</v>
+      </c>
+      <c r="K17" s="9">
+        <v>0</v>
+      </c>
+      <c r="L17" s="9">
+        <v>0</v>
+      </c>
       <c r="M17" s="9">
         <v>0</v>
       </c>
@@ -1930,12 +2062,24 @@
       <c r="F18" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
-      <c r="L18" s="9"/>
+      <c r="G18" s="9">
+        <v>0</v>
+      </c>
+      <c r="H18" s="9">
+        <v>0</v>
+      </c>
+      <c r="I18" s="9">
+        <v>0</v>
+      </c>
+      <c r="J18" s="9">
+        <v>0</v>
+      </c>
+      <c r="K18" s="9">
+        <v>0</v>
+      </c>
+      <c r="L18" s="9">
+        <v>0</v>
+      </c>
       <c r="M18" s="9">
         <v>0</v>
       </c>
@@ -1964,12 +2108,24 @@
       <c r="F19" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="9"/>
-      <c r="L19" s="9"/>
+      <c r="G19" s="9">
+        <v>0</v>
+      </c>
+      <c r="H19" s="9">
+        <v>0</v>
+      </c>
+      <c r="I19" s="9">
+        <v>0</v>
+      </c>
+      <c r="J19" s="9">
+        <v>0</v>
+      </c>
+      <c r="K19" s="9">
+        <v>0</v>
+      </c>
+      <c r="L19" s="9">
+        <v>0</v>
+      </c>
       <c r="M19" s="9">
         <v>0</v>
       </c>
@@ -2020,12 +2176,24 @@
       <c r="F21" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
-      <c r="K21" s="9"/>
-      <c r="L21" s="9"/>
+      <c r="G21" s="9">
+        <v>0</v>
+      </c>
+      <c r="H21" s="9">
+        <v>0</v>
+      </c>
+      <c r="I21" s="9">
+        <v>0</v>
+      </c>
+      <c r="J21" s="9">
+        <v>0</v>
+      </c>
+      <c r="K21" s="9">
+        <v>0</v>
+      </c>
+      <c r="L21" s="9">
+        <v>0</v>
+      </c>
       <c r="M21" s="9">
         <v>0</v>
       </c>
@@ -2054,12 +2222,24 @@
       <c r="F22" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
-      <c r="J22" s="9"/>
-      <c r="K22" s="9"/>
-      <c r="L22" s="9"/>
+      <c r="G22" s="9">
+        <v>0</v>
+      </c>
+      <c r="H22" s="9">
+        <v>0</v>
+      </c>
+      <c r="I22" s="9">
+        <v>0</v>
+      </c>
+      <c r="J22" s="9">
+        <v>0</v>
+      </c>
+      <c r="K22" s="9">
+        <v>0</v>
+      </c>
+      <c r="L22" s="9">
+        <v>0</v>
+      </c>
       <c r="M22" s="9">
         <v>0</v>
       </c>
@@ -2110,12 +2290,24 @@
       <c r="F24" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
-      <c r="J24" s="9"/>
-      <c r="K24" s="9"/>
-      <c r="L24" s="9"/>
+      <c r="G24" s="9">
+        <v>0</v>
+      </c>
+      <c r="H24" s="9">
+        <v>0</v>
+      </c>
+      <c r="I24" s="9">
+        <v>0</v>
+      </c>
+      <c r="J24" s="9">
+        <v>0</v>
+      </c>
+      <c r="K24" s="9">
+        <v>0</v>
+      </c>
+      <c r="L24" s="9">
+        <v>0</v>
+      </c>
       <c r="M24" s="9">
         <v>0</v>
       </c>
@@ -2144,12 +2336,24 @@
       <c r="F25" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="G25" s="9"/>
-      <c r="H25" s="9"/>
-      <c r="I25" s="9"/>
-      <c r="J25" s="9"/>
-      <c r="K25" s="9"/>
-      <c r="L25" s="9"/>
+      <c r="G25" s="9">
+        <v>0</v>
+      </c>
+      <c r="H25" s="9">
+        <v>0</v>
+      </c>
+      <c r="I25" s="9">
+        <v>0</v>
+      </c>
+      <c r="J25" s="9">
+        <v>0</v>
+      </c>
+      <c r="K25" s="9">
+        <v>0</v>
+      </c>
+      <c r="L25" s="9">
+        <v>0</v>
+      </c>
       <c r="M25" s="9">
         <v>0</v>
       </c>
@@ -2178,12 +2382,24 @@
       <c r="F26" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="G26" s="9"/>
-      <c r="H26" s="9"/>
-      <c r="I26" s="9"/>
-      <c r="J26" s="9"/>
-      <c r="K26" s="9"/>
-      <c r="L26" s="9"/>
+      <c r="G26" s="9">
+        <v>0</v>
+      </c>
+      <c r="H26" s="9">
+        <v>0</v>
+      </c>
+      <c r="I26" s="9">
+        <v>0</v>
+      </c>
+      <c r="J26" s="9">
+        <v>0</v>
+      </c>
+      <c r="K26" s="9">
+        <v>0</v>
+      </c>
+      <c r="L26" s="9">
+        <v>0</v>
+      </c>
       <c r="M26" s="9">
         <v>0</v>
       </c>
@@ -2212,12 +2428,24 @@
       <c r="F27" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="G27" s="9"/>
-      <c r="H27" s="9"/>
-      <c r="I27" s="9"/>
-      <c r="J27" s="9"/>
-      <c r="K27" s="9"/>
-      <c r="L27" s="9"/>
+      <c r="G27" s="9">
+        <v>0</v>
+      </c>
+      <c r="H27" s="9">
+        <v>0</v>
+      </c>
+      <c r="I27" s="9">
+        <v>0</v>
+      </c>
+      <c r="J27" s="9">
+        <v>0</v>
+      </c>
+      <c r="K27" s="9">
+        <v>0</v>
+      </c>
+      <c r="L27" s="9">
+        <v>0</v>
+      </c>
       <c r="M27" s="9">
         <v>0</v>
       </c>
@@ -2284,12 +2512,24 @@
       <c r="F29" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="G29" s="14"/>
-      <c r="H29" s="14"/>
-      <c r="I29" s="14"/>
-      <c r="J29" s="14"/>
-      <c r="K29" s="14"/>
-      <c r="L29" s="14"/>
+      <c r="G29" s="9">
+        <v>0</v>
+      </c>
+      <c r="H29" s="9">
+        <v>0</v>
+      </c>
+      <c r="I29" s="9">
+        <v>0</v>
+      </c>
+      <c r="J29" s="9">
+        <v>0</v>
+      </c>
+      <c r="K29" s="9">
+        <v>0</v>
+      </c>
+      <c r="L29" s="9">
+        <v>0</v>
+      </c>
       <c r="M29" s="14">
         <v>0</v>
       </c>
@@ -2318,12 +2558,24 @@
       <c r="F30" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="G30" s="9"/>
-      <c r="H30" s="9"/>
-      <c r="I30" s="9"/>
-      <c r="J30" s="9"/>
-      <c r="K30" s="9"/>
-      <c r="L30" s="9"/>
+      <c r="G30" s="9">
+        <v>0</v>
+      </c>
+      <c r="H30" s="9">
+        <v>0</v>
+      </c>
+      <c r="I30" s="9">
+        <v>0</v>
+      </c>
+      <c r="J30" s="9">
+        <v>0</v>
+      </c>
+      <c r="K30" s="9">
+        <v>0</v>
+      </c>
+      <c r="L30" s="9">
+        <v>0</v>
+      </c>
       <c r="M30" s="9">
         <v>0</v>
       </c>
@@ -2390,12 +2642,24 @@
       <c r="F32" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="G32" s="9"/>
-      <c r="H32" s="9"/>
-      <c r="I32" s="9"/>
-      <c r="J32" s="9"/>
-      <c r="K32" s="9"/>
-      <c r="L32" s="9"/>
+      <c r="G32" s="9">
+        <v>0</v>
+      </c>
+      <c r="H32" s="9">
+        <v>0</v>
+      </c>
+      <c r="I32" s="9">
+        <v>0</v>
+      </c>
+      <c r="J32" s="9">
+        <v>0</v>
+      </c>
+      <c r="K32" s="9">
+        <v>0</v>
+      </c>
+      <c r="L32" s="9">
+        <v>0</v>
+      </c>
       <c r="M32" s="9">
         <v>0</v>
       </c>
@@ -2424,12 +2688,24 @@
       <c r="F33" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="G33" s="14"/>
-      <c r="H33" s="14"/>
-      <c r="I33" s="14"/>
-      <c r="J33" s="14"/>
-      <c r="K33" s="14"/>
-      <c r="L33" s="14"/>
+      <c r="G33" s="9">
+        <v>0</v>
+      </c>
+      <c r="H33" s="9">
+        <v>0</v>
+      </c>
+      <c r="I33" s="9">
+        <v>0</v>
+      </c>
+      <c r="J33" s="9">
+        <v>0</v>
+      </c>
+      <c r="K33" s="9">
+        <v>0</v>
+      </c>
+      <c r="L33" s="9">
+        <v>0</v>
+      </c>
       <c r="M33" s="14">
         <v>0</v>
       </c>
@@ -2480,12 +2756,24 @@
       <c r="F35" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="G35" s="9"/>
-      <c r="H35" s="9"/>
-      <c r="I35" s="9"/>
-      <c r="J35" s="9"/>
-      <c r="K35" s="9"/>
-      <c r="L35" s="9"/>
+      <c r="G35" s="9">
+        <v>0</v>
+      </c>
+      <c r="H35" s="9">
+        <v>0</v>
+      </c>
+      <c r="I35" s="9">
+        <v>0</v>
+      </c>
+      <c r="J35" s="9">
+        <v>0</v>
+      </c>
+      <c r="K35" s="9">
+        <v>0</v>
+      </c>
+      <c r="L35" s="9">
+        <v>0</v>
+      </c>
       <c r="M35" s="9">
         <v>0</v>
       </c>
@@ -2514,12 +2802,24 @@
       <c r="F36" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="G36" s="9"/>
-      <c r="H36" s="9"/>
-      <c r="I36" s="9"/>
-      <c r="J36" s="9"/>
-      <c r="K36" s="9"/>
-      <c r="L36" s="9"/>
+      <c r="G36" s="9">
+        <v>0</v>
+      </c>
+      <c r="H36" s="9">
+        <v>0</v>
+      </c>
+      <c r="I36" s="9">
+        <v>0</v>
+      </c>
+      <c r="J36" s="9">
+        <v>0</v>
+      </c>
+      <c r="K36" s="9">
+        <v>0</v>
+      </c>
+      <c r="L36" s="9">
+        <v>0</v>
+      </c>
       <c r="M36" s="9">
         <v>0</v>
       </c>

</xml_diff>